<commit_message>
:sparkles: start build CreateTeacherAccount
</commit_message>
<xml_diff>
--- a/public/static/excels/giao-vu-example.xlsx
+++ b/public/static/excels/giao-vu-example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HoangNam\Documents\Office\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\projects\b4e_new\school\frontend\public\static\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D20B98D-4627-4D49-94CF-484F32CDAB58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0B9FF7-D744-48BD-BBFE-E1BA45B80B6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5316" yWindow="2112" windowWidth="17280" windowHeight="9072" xr2:uid="{9A2A20E7-0F4D-4070-A35D-DB446CDE88F3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{9A2A20E7-0F4D-4070-A35D-DB446CDE88F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>Viện</t>
   </si>
   <si>
-    <t>CB1234</t>
-  </si>
-  <si>
     <t>Nguyễn Văn B</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>Viện CNTT&amp;TT</t>
   </si>
   <si>
-    <t>CB1235</t>
-  </si>
-  <si>
     <t>Viện Sư phạm Kỹ thuật</t>
   </si>
   <si>
@@ -87,9 +81,6 @@
     <t>AnLpO4jxLPGUjNBpJmnOja/FpXdncPS363uMJwYnS0n9</t>
   </si>
   <si>
-    <t>CB1236</t>
-  </si>
-  <si>
     <t>Lê Thị D</t>
   </si>
   <si>
@@ -99,9 +90,6 @@
     <t>Aq7DZm5J4jBJNPMCSaEAg2qOY9icCYoigIBOLAN8WPiV</t>
   </si>
   <si>
-    <t>CB1237</t>
-  </si>
-  <si>
     <t>Trần Văn E</t>
   </si>
   <si>
@@ -111,9 +99,6 @@
     <t>AxrZLzzkIheuNY3Ff0VawaXdVAdjlGq61bUAocL/ZXgG</t>
   </si>
   <si>
-    <t>CB1238</t>
-  </si>
-  <si>
     <t>Đào Thị F</t>
   </si>
   <si>
@@ -124,6 +109,21 @@
   </si>
   <si>
     <t>A22V6uhd9uFISY7IcQshKuJ5sEBMuoORHqsTYL5gHQav</t>
+  </si>
+  <si>
+    <t>Gvu1234</t>
+  </si>
+  <si>
+    <t>Gvu1235</t>
+  </si>
+  <si>
+    <t>Gvu1236</t>
+  </si>
+  <si>
+    <t>Gvu1237</t>
+  </si>
+  <si>
+    <t>Gvu1238</t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A6" sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,7 +493,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -505,92 +505,92 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:construction: testing, refine, tuning...
</commit_message>
<xml_diff>
--- a/public/static/excels/giao-vu-example.xlsx
+++ b/public/static/excels/giao-vu-example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HoangNam\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\projects\b4e_new\school\frontend\public\static\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80F916B-EC51-410F-A19C-89CB966E4241}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB7F25B-C00E-4475-9F05-DA1B6DA53032}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{6F060DE9-65CA-46F3-A880-71911037B99D}"/>
   </bookViews>
@@ -54,45 +54,30 @@
     <t>Nguyễn Văn B</t>
   </si>
   <si>
-    <t>nguyenvanb@soict.hust.edu.vn</t>
-  </si>
-  <si>
     <t>Viện CNTT&amp;TT</t>
   </si>
   <si>
     <t>Lý Thị C</t>
   </si>
   <si>
-    <t>lythic@spkt.hust.edu.vn</t>
-  </si>
-  <si>
     <t>Viện Sư phạm Kỹ thuật</t>
   </si>
   <si>
     <t>Lê Thị D</t>
   </si>
   <si>
-    <t>lethidc@nn.hust.edu.vn</t>
-  </si>
-  <si>
     <t>Viện Ngoại ngữ</t>
   </si>
   <si>
     <t>Trần Văn E</t>
   </si>
   <si>
-    <t>tranvane@dtvt.hust.edu.vn</t>
-  </si>
-  <si>
     <t>Viện Điện tử viễn thông</t>
   </si>
   <si>
     <t>Đào Thị F</t>
   </si>
   <si>
-    <t>daothif@dktdh.hust.edu.vn</t>
-  </si>
-  <si>
     <t>Viện Điều khiển Tự động hóa</t>
   </si>
   <si>
@@ -124,16 +109,39 @@
   </si>
   <si>
     <t>9f8d8cebb1757c48b23052c10e2d80bf68f9f96fc22fb2aa1e88ec2091a3cb5c17f2a9742f37e93bc10df6cf83698d8c26e14402f190a09f5fba659115421088</t>
+  </si>
+  <si>
+    <t>nguyenvanb@gvu.soict.hust.edu.vn</t>
+  </si>
+  <si>
+    <t>lythic@gvu.spkt.hust.edu.vn</t>
+  </si>
+  <si>
+    <t>lethidc@gvu.nn.hust.edu.vn</t>
+  </si>
+  <si>
+    <t>tranvane@gvu.dtvt.hust.edu.vn</t>
+  </si>
+  <si>
+    <t>daothif@gvu.dktdh.hust.edu.vn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -156,13 +164,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -478,7 +489,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,91 +520,98 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{011B2361-D359-437E-9600-6230ECBB300F}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{D6BF299F-3F73-4A50-94DA-3C02E935DAD4}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{320CCF2E-82FE-454A-84FE-C5BF1DA01D8D}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{7AD9EAEA-867F-4DD2-A1E5-E4DE22C2889C}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{286AB299-531E-4D42-827B-1628E55E24F8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>